<commit_message>
Tracing & legend now on same sheet. Removed TOC.
</commit_message>
<xml_diff>
--- a/traceur.xlsx
+++ b/traceur.xlsx
@@ -1,41 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F17D10-4B6E-4B7D-BD2A-5CE9A9D62D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="14265" yWindow="3405" windowWidth="21855" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Export Summary" sheetId="1" r:id="rId4"/>
-    <sheet name="Sheet 1 - Contact Tracing" sheetId="2" r:id="rId5"/>
-    <sheet name="Sheet 1 - Legend" sheetId="3" r:id="rId6"/>
+    <sheet name="Contact Tracing" sheetId="2" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
-  <si>
-    <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
-  </si>
-  <si>
-    <t>Numbers Sheet Name</t>
-  </si>
-  <si>
-    <t>Numbers Table Name</t>
-  </si>
-  <si>
-    <t>Excel Worksheet Name</t>
-  </si>
-  <si>
-    <t>Sheet 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
   <si>
     <t>Contact Tracing</t>
   </si>
   <si>
-    <t>Sheet 1 - Contact Tracing</t>
-  </si>
-  <si>
     <t>Person 1</t>
   </si>
   <si>
@@ -85,9 +69,6 @@
   </si>
   <si>
     <t>Legend</t>
-  </si>
-  <si>
-    <t>Sheet 1 - Legend</t>
   </si>
   <si>
     <t>Symbol</t>
@@ -153,41 +134,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="m/d"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="12"/>
-      <color indexed="11"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="16"/>
       <color indexed="8"/>
       <name val="Avenir Next Regular"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="12"/>
       <name val="Avenir Next Regular"/>
@@ -198,7 +162,7 @@
       <name val="Avenir Next Regular"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Avenir Next Regular"/>
@@ -209,24 +173,12 @@
       <name val="Avenir Next Regular"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor auto="1"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -308,85 +260,67 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="6" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="6" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="7" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -396,31 +330,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="015e88b1"/>
-      <rgbColor rgb="01eef3f4"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="fffefffe"/>
-      <rgbColor rgb="ff00a1fe"/>
-      <rgbColor rgb="ffc8c8c8"/>
-      <rgbColor rgb="ff89847f"/>
-      <rgbColor rgb="fff7f7f6"/>
-      <rgbColor rgb="fffff056"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="015E88B1"/>
+      <rgbColor rgb="01EEF3F4"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFEFFFE"/>
+      <rgbColor rgb="FF00A1FE"/>
+      <rgbColor rgb="FFC8C8C8"/>
+      <rgbColor rgb="FF89847F"/>
+      <rgbColor rgb="FFF7F7F6"/>
+      <rgbColor rgb="FFFFF056"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -619,7 +607,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -638,7 +626,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -668,7 +656,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -694,7 +682,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -720,7 +708,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -746,7 +734,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -772,7 +760,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -798,7 +786,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -824,7 +812,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -850,7 +838,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -876,7 +864,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -889,9 +877,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -908,7 +902,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -927,7 +921,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -953,7 +947,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -979,7 +973,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1005,7 +999,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1031,7 +1025,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1057,7 +1051,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1083,7 +1077,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1109,7 +1103,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1135,7 +1129,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1161,7 +1155,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1174,9 +1168,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1190,7 +1190,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1209,7 +1209,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1239,7 +1239,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1265,7 +1265,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1291,7 +1291,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1317,7 +1317,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1343,7 +1343,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1369,7 +1369,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1395,7 +1395,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1421,7 +1421,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1447,7 +1447,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1460,528 +1460,423 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:R12"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:O1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="2" max="15" width="8" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+    <row r="1" spans="1:18" ht="36" customHeight="1">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="Q1" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="18"/>
     </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+    <row r="2" spans="1:18" ht="27.75" customHeight="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3">
+        <v>44021</v>
+      </c>
+      <c r="C2" s="4">
+        <v>44022</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44023</v>
+      </c>
+      <c r="E2" s="4">
+        <v>44024</v>
+      </c>
+      <c r="F2" s="4">
+        <v>44025</v>
+      </c>
+      <c r="G2" s="4">
+        <v>44026</v>
+      </c>
+      <c r="H2" s="4">
+        <v>44027</v>
+      </c>
+      <c r="I2" s="4">
+        <v>44028</v>
+      </c>
+      <c r="J2" s="4">
+        <v>44029</v>
+      </c>
+      <c r="K2" s="4">
+        <v>44030</v>
+      </c>
+      <c r="L2" s="4">
+        <v>44031</v>
+      </c>
+      <c r="M2" s="4">
+        <v>44032</v>
+      </c>
+      <c r="N2" s="4">
+        <v>44033</v>
+      </c>
+      <c r="O2" s="4">
+        <v>44034</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="27.6" customHeight="1">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="K3" s="8" t="s">
         <v>3</v>
       </c>
+      <c r="L3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+    <row r="4" spans="1:18" ht="27.6" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+    <row r="5" spans="1:18" ht="27.6" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="E5" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="N5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" s="16" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="11">
-      <c r="B11" s="4"/>
-      <c r="C11" t="s" s="4">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s" s="5">
-        <v>24</v>
+    <row r="6" spans="1:18" ht="27.6" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="27.6" customHeight="1">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="27.6" customHeight="1">
+      <c r="A8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="Q8" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="R8" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="27.6" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="Q9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="R9" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="27.6" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="27.6" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="Q11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="19.899999999999999" customHeight="1">
+      <c r="Q12" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="R12" s="17" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:D3"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="D10" location="'Sheet 1 - Contact Tracing'!R2C1" tooltip="" display="Sheet 1 - Contact Tracing"/>
-    <hyperlink ref="D11" location="'Sheet 1 - Legend'!R2C1" tooltip="" display="Sheet 1 - Legend"/>
-  </hyperlinks>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:O11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B1" xSplit="1" ySplit="0" activePane="topRight" state="frozen"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="10.7031" style="6" customWidth="1"/>
-    <col min="2" max="15" width="8" style="6" customWidth="1"/>
-    <col min="16" max="16384" width="16.3516" style="6" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="36" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" ht="27.75" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9">
-        <v>44021</v>
-      </c>
-      <c r="C2" s="10">
-        <v>44022</v>
-      </c>
-      <c r="D2" s="10">
-        <v>44023</v>
-      </c>
-      <c r="E2" s="10">
-        <v>44024</v>
-      </c>
-      <c r="F2" s="10">
-        <v>44025</v>
-      </c>
-      <c r="G2" s="10">
-        <v>44026</v>
-      </c>
-      <c r="H2" s="10">
-        <v>44027</v>
-      </c>
-      <c r="I2" s="10">
-        <v>44028</v>
-      </c>
-      <c r="J2" s="10">
-        <v>44029</v>
-      </c>
-      <c r="K2" s="10">
-        <v>44030</v>
-      </c>
-      <c r="L2" s="10">
-        <v>44031</v>
-      </c>
-      <c r="M2" s="10">
-        <v>44032</v>
-      </c>
-      <c r="N2" s="10">
-        <v>44033</v>
-      </c>
-      <c r="O2" s="10">
-        <v>44034</v>
-      </c>
-    </row>
-    <row r="3" ht="27.5" customHeight="1">
-      <c r="A3" t="s" s="11">
-        <v>7</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" t="s" s="14">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s" s="14">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s" s="14">
-        <v>9</v>
-      </c>
-      <c r="M3" t="s" s="14">
-        <v>9</v>
-      </c>
-      <c r="N3" t="s" s="14">
-        <v>9</v>
-      </c>
-      <c r="O3" t="s" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" ht="27.5" customHeight="1">
-      <c r="A4" t="s" s="11">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s" s="15">
-        <v>11</v>
-      </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" t="s" s="18">
-        <v>12</v>
-      </c>
-      <c r="M4" t="s" s="18">
-        <v>9</v>
-      </c>
-      <c r="N4" t="s" s="18">
-        <v>9</v>
-      </c>
-      <c r="O4" t="s" s="18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" ht="27.5" customHeight="1">
-      <c r="A5" t="s" s="11">
-        <v>13</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="E5" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="F5" s="16"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" t="s" s="19">
-        <v>14</v>
-      </c>
-      <c r="L5" t="s" s="14">
-        <v>9</v>
-      </c>
-      <c r="M5" t="s" s="14">
-        <v>12</v>
-      </c>
-      <c r="N5" t="s" s="14">
-        <v>9</v>
-      </c>
-      <c r="O5" t="s" s="14">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" ht="27.5" customHeight="1">
-      <c r="A6" t="s" s="11">
-        <v>15</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="17"/>
-      <c r="D6" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" t="s" s="19">
-        <v>14</v>
-      </c>
-      <c r="L6" t="s" s="18">
-        <v>9</v>
-      </c>
-      <c r="M6" t="s" s="18">
-        <v>9</v>
-      </c>
-      <c r="N6" t="s" s="18">
-        <v>9</v>
-      </c>
-      <c r="O6" t="s" s="18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" ht="27.5" customHeight="1">
-      <c r="A7" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" t="s" s="14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" ht="27.5" customHeight="1">
-      <c r="A8" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-    </row>
-    <row r="9" ht="27.5" customHeight="1">
-      <c r="A9" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-    </row>
-    <row r="10" ht="27.5" customHeight="1">
-      <c r="A10" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" t="s" s="19">
-        <v>20</v>
-      </c>
-      <c r="L10" t="s" s="19">
-        <v>9</v>
-      </c>
-      <c r="M10" t="s" s="18">
-        <v>9</v>
-      </c>
-      <c r="N10" t="s" s="18">
-        <v>9</v>
-      </c>
-      <c r="O10" t="s" s="18">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" ht="27.5" customHeight="1">
-      <c r="A11" t="s" s="11">
-        <v>22</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" t="s" s="19">
-        <v>11</v>
-      </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
-  </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="8.28125" style="21" customWidth="1"/>
-    <col min="2" max="2" width="27.1406" style="21" customWidth="1"/>
-    <col min="3" max="16384" width="16.3516" style="21" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="36" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>23</v>
-      </c>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" ht="27.8" customHeight="1">
-      <c r="A2" t="s" s="22">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s" s="22">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" ht="28.3" customHeight="1">
-      <c r="A3" t="s" s="14">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s" s="23">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" ht="28.3" customHeight="1">
-      <c r="A4" t="s" s="18">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s" s="24">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" ht="28.3" customHeight="1">
-      <c r="A5" t="s" s="14">
-        <v>30</v>
-      </c>
-      <c r="B5" t="s" s="23">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" ht="28.3" customHeight="1">
-      <c r="A6" t="s" s="18">
-        <v>32</v>
-      </c>
-      <c r="B6" t="s" s="24">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" ht="28.3" customHeight="1">
-      <c r="A7" s="16"/>
-      <c r="B7" t="s" s="23">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" ht="28.3" customHeight="1">
-      <c r="A8" t="s" s="18">
-        <v>35</v>
-      </c>
-      <c r="B8" t="s" s="24">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" ht="28.3" customHeight="1">
-      <c r="A9" t="s" s="14">
-        <v>37</v>
-      </c>
-      <c r="B9" t="s" s="23">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" ht="28.3" customHeight="1">
-      <c r="A10" t="s" s="18">
-        <v>39</v>
-      </c>
-      <c r="B10" t="s" s="24">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" ht="28.3" customHeight="1">
-      <c r="A11" t="s" s="14">
-        <v>41</v>
-      </c>
-      <c r="B11" t="s" s="23">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" ht="28.3" customHeight="1">
-      <c r="A12" t="s" s="18">
-        <v>43</v>
-      </c>
-      <c r="B12" t="s" s="24">
-        <v>44</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup scale="72" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Legend text no longer forces some cells taller
</commit_message>
<xml_diff>
--- a/traceur.xlsx
+++ b/traceur.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F17D10-4B6E-4B7D-BD2A-5CE9A9D62D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAE3F84-4121-405D-8CE8-58399EC70028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14265" yWindow="3405" windowWidth="21855" windowHeight="14010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14265" yWindow="3405" windowWidth="20505" windowHeight="12465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact Tracing" sheetId="2" r:id="rId1"/>
@@ -1483,15 +1483,17 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:O1"/>
+      <selection pane="topRight" activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
     <col min="2" max="15" width="8" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="16.28515625" style="1"/>
+    <col min="16" max="16" width="6.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" style="1"/>
+    <col min="18" max="18" width="27.28515625" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="16.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="36" customHeight="1">

</xml_diff>

<commit_message>
Use + and - over color emoji
Fixes #3
</commit_message>
<xml_diff>
--- a/traceur.xlsx
+++ b/traceur.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAE3F84-4121-405D-8CE8-58399EC70028}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A279D05C-BBCE-E943-8F73-1734139B13B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14265" yWindow="3405" windowWidth="20505" windowHeight="12465" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contact Tracing" sheetId="2" r:id="rId1"/>
@@ -23,9 +23,6 @@
     <t>Person 1</t>
   </si>
   <si>
-    <t>🧪⏱🔴</t>
-  </si>
-  <si>
     <t>🧬⏳</t>
   </si>
   <si>
@@ -35,9 +32,6 @@
     <t>🤚</t>
   </si>
   <si>
-    <t>⏱🟢</t>
-  </si>
-  <si>
     <t>Person 3</t>
   </si>
   <si>
@@ -59,12 +53,6 @@
     <t>Person 8</t>
   </si>
   <si>
-    <t>🧪💊🟢</t>
-  </si>
-  <si>
-    <t>🧬🟢</t>
-  </si>
-  <si>
     <t>Person 9</t>
   </si>
   <si>
@@ -80,15 +68,9 @@
     <t>Physical Contact</t>
   </si>
   <si>
-    <t>🔴</t>
-  </si>
-  <si>
     <t>Positive Test Result</t>
   </si>
   <si>
-    <t>🟢</t>
-  </si>
-  <si>
     <t>Negative Test Result</t>
   </si>
   <si>
@@ -129,6 +111,24 @@
   </si>
   <si>
     <t>Antigen Test</t>
+  </si>
+  <si>
+    <t>➖</t>
+  </si>
+  <si>
+    <t>⏱➖</t>
+  </si>
+  <si>
+    <t>🧬➖</t>
+  </si>
+  <si>
+    <t>🧪💊➖</t>
+  </si>
+  <si>
+    <t>➕</t>
+  </si>
+  <si>
+    <t>🧪⏱➕</t>
   </si>
 </sst>
 </file>
@@ -1483,17 +1483,17 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R3" sqref="R3"/>
+      <selection pane="topRight" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
     <col min="2" max="15" width="8" style="1" customWidth="1"/>
-    <col min="16" max="16" width="6.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" style="1"/>
-    <col min="18" max="18" width="27.28515625" style="1" customWidth="1"/>
-    <col min="19" max="16384" width="16.28515625" style="1"/>
+    <col min="16" max="16" width="6.5" style="1" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" style="1"/>
+    <col min="18" max="18" width="27.33203125" style="1" customWidth="1"/>
+    <col min="19" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="36" customHeight="1">
@@ -1515,7 +1515,7 @@
       <c r="N1" s="18"/>
       <c r="O1" s="18"/>
       <c r="Q1" s="18" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="R1" s="18"/>
     </row>
@@ -1564,13 +1564,13 @@
         <v>44034</v>
       </c>
       <c r="Q2" s="15" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="27.6" customHeight="1">
+    <row r="3" spans="1:18" ht="27.5" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -1583,36 +1583,36 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="27.5" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="27.6" customHeight="1">
-      <c r="A4" s="5" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>5</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -1624,35 +1624,35 @@
       <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="12" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N4" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O4" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="12" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="27.6" customHeight="1">
+    <row r="5" spans="1:18" ht="27.5" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="7"/>
       <c r="D5" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -1660,38 +1660,38 @@
       <c r="I5" s="10"/>
       <c r="J5" s="10"/>
       <c r="K5" s="13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="R5" s="16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="27.6" customHeight="1">
+    <row r="6" spans="1:18" ht="27.5" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="14"/>
       <c r="C6" s="11"/>
       <c r="D6" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -1699,36 +1699,36 @@
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="27.5" customHeight="1">
+      <c r="A7" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="L6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="M6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O6" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="R6" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="27.6" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>10</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
@@ -1740,22 +1740,22 @@
       <c r="M7" s="7"/>
       <c r="N7" s="7"/>
       <c r="O7" s="8" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="Q7" s="10"/>
       <c r="R7" s="16" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="27.6" customHeight="1">
+    <row r="8" spans="1:18" ht="27.5" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="14"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
@@ -1768,21 +1768,21 @@
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
       <c r="Q8" s="12" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="R8" s="17" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="27.6" customHeight="1">
+    <row r="9" spans="1:18" ht="27.5" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
@@ -1795,59 +1795,59 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="Q9" s="8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="R9" s="16" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="27.6" customHeight="1">
+    <row r="10" spans="1:18" ht="27.5" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="13" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="27.6" customHeight="1">
+    <row r="11" spans="1:18" ht="27.5" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
@@ -1859,18 +1859,18 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="Q11" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="R11" s="16" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="19.899999999999999" customHeight="1">
+    <row r="12" spans="1:18" ht="20" customHeight="1">
       <c r="Q12" s="12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>